<commit_message>
Gerenciamento de riscos tabela
TABELA COM TODOS POSSIVEIS RISCOS DE PROJETO
</commit_message>
<xml_diff>
--- a/gerenciamento/TABELA GERENCIAMENTO DE RISCOS.xlsx
+++ b/gerenciamento/TABELA GERENCIAMENTO DE RISCOS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Formulário de informações do risco</t>
   </si>
@@ -1063,6 +1063,259 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">R$ 29.920,9 </t>
+    </r>
+  </si>
+  <si>
+    <t>Evento: 005</t>
+  </si>
+  <si>
+    <t>Probabilidade: 75%</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Descrição:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Risco de cronograma o planejamento realizado não atendeu as expectativas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Subcondição 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Planejamento realizado está fora do idealizado</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subcondição 3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Planejamento fora do esperado</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Subcondição 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Outras equipes não cumprem com os prazos estabelecidos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sub. 2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reunião com as equipes para colocar um novo cronograma em dia com todas as atividades definidas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sub. 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Equipe deve verificar onde estão possiveis erros no planejamento apresentando soluções</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sub. 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Equipe de planejamento deve realizar novo cronograma </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Caso 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Valor cobrado pelo tempo gasto para realizar verificação dos requisitos pela equipe atrasando outros componentes do projeto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R$ 1.838,97</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Caso 2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Valor cobrado por 2 dias para realizar reuniao com todos membros da equipe  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R$ 2.162,42</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Caso 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Valor cobrado pelo tempo gasto da equipe com um novo planejamento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">R$ 42.167,4 </t>
     </r>
   </si>
 </sst>
@@ -1295,97 +1548,95 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1413,6 +1664,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1704,235 +1957,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="35" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -2112,235 +2365,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="35" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -2493,11 +2746,6 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:H27"/>
     <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:H16"/>
-    <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H20"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
@@ -2505,12 +2753,17 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A4:H5"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2520,235 +2773,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="35" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="42"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="50"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -2901,11 +3154,6 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:H27"/>
     <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:H16"/>
-    <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H20"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
@@ -2913,12 +3161,17 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A4:H5"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2928,93 +3181,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="35" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
@@ -3029,36 +3282,36 @@
       <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
@@ -3073,90 +3326,90 @@
       <c r="H12" s="53"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -3309,11 +3562,6 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:H27"/>
     <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:H16"/>
-    <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H20"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
@@ -3321,12 +3569,17 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A4:H5"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3336,97 +3589,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="35"/>
+      <c r="A2" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="A4" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -3437,40 +3690,40 @@
       <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="A10" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B12" s="53"/>
       <c r="C12" s="53"/>
@@ -3481,90 +3734,90 @@
       <c r="H12" s="53"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="A15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
+      <c r="A18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -3578,7 +3831,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3622,7 +3875,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -3654,7 +3907,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3686,7 +3939,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3717,11 +3970,6 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:H27"/>
     <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:H16"/>
-    <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H20"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
@@ -3729,13 +3977,19 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A4:H5"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>